<commit_message>
feat: add Python OOP concept examples
</commit_message>
<xml_diff>
--- a/09_wa_automation/contact.xlsx
+++ b/09_wa_automation/contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\09_wa_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17F70C5-801B-4818-8D07-44D42C4DCC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3C8116-CFBA-49E0-99EF-A77D61FDA62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70EECB6D-9290-4491-BC12-C3E9C28FCD8B}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +426,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7079685322</v>
+        <v>7857831014</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
feat: update WhatsApp message template, enhance file handling, and add threading examples
</commit_message>
<xml_diff>
--- a/09_wa_automation/contact.xlsx
+++ b/09_wa_automation/contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\09_wa_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3C8116-CFBA-49E0-99EF-A77D61FDA62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3897DB6-93E2-4DF2-81B1-B105CAA2E7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70EECB6D-9290-4491-BC12-C3E9C28FCD8B}"/>
   </bookViews>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Number</t>
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Rupesh So</t>
   </si>
   <si>
     <t>Rupesh</t>
@@ -397,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F733F8B-6E32-4628-AF07-2CE8DFEC0037}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -418,18 +415,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8235068541</v>
+        <v>1234567890</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>7857831014</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>